<commit_message>
small changes and notes
</commit_message>
<xml_diff>
--- a/Mouse_workbooks/CH_050614_B.xlsx
+++ b/Mouse_workbooks/CH_050614_B.xlsx
@@ -300,9 +300,6 @@
     <t>Steps at (-170 267). Looking at spatial spread. Repeats of 10 volts pulses. Little response here. Some failures.</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>2014_05_19_0024</t>
   </si>
   <si>
@@ -334,6 +331,9 @@
   </si>
   <si>
     <t>Two recordings, from the same slice, hoepfully AL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trains, 5 Hz, at (-91 330), FS closed.. Much weaker responses than at the soma. </t>
   </si>
 </sst>
 </file>
@@ -976,15 +976,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -994,6 +985,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1084,32 +1084,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1544,8 +1544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:H4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="56"/>
       <c r="E1" s="56"/>
@@ -1584,12 +1584,12 @@
         <v>8</v>
       </c>
       <c r="B2" s="52"/>
-      <c r="C2" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="C2" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="26" t="s">
         <v>30</v>
       </c>
@@ -1605,9 +1605,9 @@
       <c r="C3" s="42">
         <v>34</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="43"/>
       <c r="H3" s="44"/>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B4" s="54"/>
       <c r="C4" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" s="46"/>
       <c r="E4" s="46"/>
@@ -1651,11 +1651,11 @@
       <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -1663,9 +1663,9 @@
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="23"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="40"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
     </row>
     <row r="8" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1681,11 +1681,11 @@
       <c r="E8" s="23">
         <v>-79</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
     </row>
     <row r="9" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -1701,11 +1701,11 @@
       <c r="E9" s="23">
         <v>-79</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1721,11 +1721,11 @@
       <c r="E10" s="23">
         <v>-85</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -1741,11 +1741,11 @@
       <c r="E11" s="34">
         <v>-85</v>
       </c>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="40"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -1761,11 +1761,11 @@
       <c r="E12" s="34">
         <v>-85</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -1781,11 +1781,11 @@
       <c r="E13" s="34">
         <v>-85</v>
       </c>
-      <c r="F13" s="38" t="s">
+      <c r="F13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="39"/>
-      <c r="H13" s="40"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
     </row>
     <row r="14" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -1801,11 +1801,11 @@
       <c r="E14" s="34">
         <v>-85</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="39"/>
-      <c r="H14" s="40"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1821,11 +1821,11 @@
       <c r="E15" s="34">
         <v>-85</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="39"/>
-      <c r="H15" s="40"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -1841,11 +1841,11 @@
       <c r="E16" s="34">
         <v>-85</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
     </row>
     <row r="17" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -1861,11 +1861,11 @@
       <c r="E17" s="34">
         <v>-85</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="39"/>
-      <c r="H17" s="40"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
     </row>
     <row r="18" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1881,11 +1881,11 @@
       <c r="E18" s="34">
         <v>-85</v>
       </c>
-      <c r="F18" s="38" t="s">
+      <c r="F18" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="39"/>
-      <c r="H18" s="40"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
     <row r="19" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -1901,11 +1901,11 @@
       <c r="E19" s="34">
         <v>-85</v>
       </c>
-      <c r="F19" s="38" t="s">
+      <c r="F19" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
     </row>
     <row r="20" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -1921,11 +1921,11 @@
       <c r="E20" s="23">
         <v>-85</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="F20" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="40"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
     </row>
     <row r="21" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -1937,11 +1937,11 @@
       <c r="E21" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="38" t="s">
+      <c r="F21" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="39"/>
-      <c r="H21" s="40"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
     </row>
     <row r="22" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -1949,9 +1949,9 @@
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
       <c r="E22" s="23"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="40"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
     </row>
     <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -1959,9 +1959,9 @@
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
       <c r="E23" s="23"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="40"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
     </row>
     <row r="24" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -1977,11 +1977,11 @@
       <c r="E24" s="23">
         <v>-72</v>
       </c>
-      <c r="F24" s="38" t="s">
+      <c r="F24" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G24" s="39"/>
-      <c r="H24" s="40"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
     </row>
     <row r="25" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
@@ -1997,11 +1997,11 @@
       <c r="E25" s="23">
         <v>-74</v>
       </c>
-      <c r="F25" s="38" t="s">
+      <c r="F25" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="G25" s="39"/>
-      <c r="H25" s="40"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
     </row>
     <row r="26" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
@@ -2017,11 +2017,11 @@
       <c r="E26" s="23">
         <v>-85</v>
       </c>
-      <c r="F26" s="38" t="s">
+      <c r="F26" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="39"/>
-      <c r="H26" s="40"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
     </row>
     <row r="27" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -2037,11 +2037,11 @@
       <c r="E27" s="34">
         <v>-85</v>
       </c>
-      <c r="F27" s="38" t="s">
+      <c r="F27" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
     </row>
     <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
@@ -2057,11 +2057,11 @@
       <c r="E28" s="34">
         <v>-85</v>
       </c>
-      <c r="F28" s="38" t="s">
+      <c r="F28" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="G28" s="39"/>
-      <c r="H28" s="40"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
     </row>
     <row r="29" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
@@ -2077,11 +2077,11 @@
       <c r="E29" s="34">
         <v>-85</v>
       </c>
-      <c r="F29" s="38" t="s">
+      <c r="F29" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G29" s="39"/>
-      <c r="H29" s="40"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
     </row>
     <row r="30" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -2097,11 +2097,11 @@
       <c r="E30" s="34">
         <v>-85</v>
       </c>
-      <c r="F30" s="38" t="s">
+      <c r="F30" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="39"/>
-      <c r="H30" s="40"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
     </row>
     <row r="31" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -2117,11 +2117,11 @@
       <c r="E31" s="34">
         <v>-85</v>
       </c>
-      <c r="F31" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" s="39"/>
-      <c r="H31" s="40"/>
+      <c r="F31" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="36"/>
+      <c r="H31" s="37"/>
     </row>
     <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -2137,11 +2137,11 @@
       <c r="E32" s="34">
         <v>-85</v>
       </c>
-      <c r="F32" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="G32" s="39"/>
-      <c r="H32" s="40"/>
+      <c r="F32" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" s="36"/>
+      <c r="H32" s="37"/>
     </row>
     <row r="33" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -2157,11 +2157,11 @@
       <c r="E33" s="34">
         <v>-85</v>
       </c>
-      <c r="F33" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="G33" s="39"/>
-      <c r="H33" s="40"/>
+      <c r="F33" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" s="36"/>
+      <c r="H33" s="37"/>
     </row>
     <row r="34" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
@@ -2177,18 +2177,18 @@
       <c r="E34" s="34">
         <v>-85</v>
       </c>
-      <c r="F34" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="G34" s="39"/>
-      <c r="H34" s="40"/>
+      <c r="F34" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="36"/>
+      <c r="H34" s="37"/>
     </row>
     <row r="35" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>2</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>41</v>
@@ -2197,18 +2197,18 @@
       <c r="E35" s="34">
         <v>-85</v>
       </c>
-      <c r="F35" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="G35" s="39"/>
-      <c r="H35" s="40"/>
+      <c r="F35" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="G35" s="36"/>
+      <c r="H35" s="37"/>
     </row>
     <row r="36" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>2</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>41</v>
@@ -2217,18 +2217,18 @@
       <c r="E36" s="34">
         <v>-85</v>
       </c>
-      <c r="F36" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="G36" s="39"/>
-      <c r="H36" s="40"/>
+      <c r="F36" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="G36" s="36"/>
+      <c r="H36" s="37"/>
     </row>
     <row r="37" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>2</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>41</v>
@@ -2237,11 +2237,11 @@
       <c r="E37" s="34">
         <v>-85</v>
       </c>
-      <c r="F37" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="G37" s="39"/>
-      <c r="H37" s="40"/>
+      <c r="F37" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" s="36"/>
+      <c r="H37" s="37"/>
     </row>
     <row r="38" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
@@ -2253,11 +2253,11 @@
       <c r="E38" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="F38" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="G38" s="39"/>
-      <c r="H38" s="40"/>
+      <c r="F38" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" s="36"/>
+      <c r="H38" s="37"/>
     </row>
     <row r="39" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
@@ -2265,9 +2265,9 @@
       <c r="C39" s="4"/>
       <c r="D39" s="5"/>
       <c r="E39" s="23"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="40"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="37"/>
     </row>
     <row r="40" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
@@ -2275,9 +2275,9 @@
       <c r="C40" s="4"/>
       <c r="D40" s="5"/>
       <c r="E40" s="23"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="40"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="37"/>
     </row>
     <row r="41" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
@@ -2285,9 +2285,9 @@
       <c r="C41" s="4"/>
       <c r="D41" s="5"/>
       <c r="E41" s="23"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="40"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="37"/>
     </row>
     <row r="42" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
@@ -2295,9 +2295,9 @@
       <c r="C42" s="4"/>
       <c r="D42" s="5"/>
       <c r="E42" s="23"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="40"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
     </row>
     <row r="43" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
@@ -2305,9 +2305,9 @@
       <c r="C43" s="4"/>
       <c r="D43" s="5"/>
       <c r="E43" s="23"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="40"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="37"/>
     </row>
     <row r="44" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
@@ -2315,9 +2315,9 @@
       <c r="C44" s="4"/>
       <c r="D44" s="5"/>
       <c r="E44" s="23"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="40"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="37"/>
     </row>
     <row r="45" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
@@ -2325,9 +2325,9 @@
       <c r="C45" s="4"/>
       <c r="D45" s="5"/>
       <c r="E45" s="23"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="40"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="37"/>
     </row>
     <row r="46" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
@@ -2335,9 +2335,9 @@
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
       <c r="E46" s="23"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="40"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="37"/>
     </row>
     <row r="47" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
@@ -2345,9 +2345,9 @@
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
       <c r="E47" s="23"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="40"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="37"/>
     </row>
     <row r="48" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
@@ -2355,9 +2355,9 @@
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
       <c r="E48" s="23"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="40"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="37"/>
     </row>
     <row r="49" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
@@ -2365,9 +2365,9 @@
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
       <c r="E49" s="23"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="40"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="37"/>
     </row>
     <row r="50" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
@@ -2375,9 +2375,9 @@
       <c r="C50" s="4"/>
       <c r="D50" s="5"/>
       <c r="E50" s="23"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="40"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="37"/>
     </row>
     <row r="51" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
@@ -2385,9 +2385,9 @@
       <c r="C51" s="4"/>
       <c r="D51" s="5"/>
       <c r="E51" s="23"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="40"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="37"/>
     </row>
     <row r="52" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
@@ -2395,9 +2395,9 @@
       <c r="C52" s="4"/>
       <c r="D52" s="5"/>
       <c r="E52" s="23"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="40"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="37"/>
     </row>
     <row r="53" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
@@ -2405,9 +2405,9 @@
       <c r="C53" s="4"/>
       <c r="D53" s="5"/>
       <c r="E53" s="23"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="40"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="37"/>
     </row>
     <row r="54" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
@@ -2415,9 +2415,9 @@
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
       <c r="E54" s="23"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="40"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="37"/>
     </row>
     <row r="55" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
@@ -2425,9 +2425,9 @@
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
       <c r="E55" s="23"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="40"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="37"/>
     </row>
     <row r="56" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
@@ -2435,9 +2435,9 @@
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
       <c r="E56" s="23"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="39"/>
-      <c r="H56" s="40"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="37"/>
     </row>
     <row r="57" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
@@ -2445,9 +2445,9 @@
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
       <c r="E57" s="23"/>
-      <c r="F57" s="38"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="40"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="37"/>
     </row>
     <row r="58" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
@@ -2455,9 +2455,9 @@
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
       <c r="E58" s="23"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="40"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="36"/>
+      <c r="H58" s="37"/>
     </row>
     <row r="59" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
@@ -2465,9 +2465,9 @@
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
       <c r="E59" s="23"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="40"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="37"/>
     </row>
     <row r="60" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
@@ -2475,9 +2475,9 @@
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
       <c r="E60" s="23"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="40"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="37"/>
     </row>
     <row r="61" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
@@ -2485,9 +2485,9 @@
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
       <c r="E61" s="23"/>
-      <c r="F61" s="38"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="40"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="36"/>
+      <c r="H61" s="37"/>
     </row>
     <row r="62" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
@@ -2495,9 +2495,9 @@
       <c r="C62" s="4"/>
       <c r="D62" s="5"/>
       <c r="E62" s="23"/>
-      <c r="F62" s="38"/>
-      <c r="G62" s="39"/>
-      <c r="H62" s="40"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="37"/>
     </row>
     <row r="63" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
@@ -2505,9 +2505,9 @@
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
       <c r="E63" s="23"/>
-      <c r="F63" s="38"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="40"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="37"/>
     </row>
     <row r="64" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
@@ -2515,9 +2515,9 @@
       <c r="C64" s="4"/>
       <c r="D64" s="5"/>
       <c r="E64" s="23"/>
-      <c r="F64" s="38"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="40"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="37"/>
     </row>
     <row r="65" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
@@ -2525,9 +2525,9 @@
       <c r="C65" s="4"/>
       <c r="D65" s="5"/>
       <c r="E65" s="23"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="40"/>
+      <c r="F65" s="35"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="37"/>
     </row>
     <row r="66" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
@@ -2535,9 +2535,9 @@
       <c r="C66" s="4"/>
       <c r="D66" s="5"/>
       <c r="E66" s="23"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="40"/>
+      <c r="F66" s="35"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="37"/>
     </row>
     <row r="67" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
@@ -2545,9 +2545,9 @@
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
       <c r="E67" s="23"/>
-      <c r="F67" s="38"/>
-      <c r="G67" s="39"/>
-      <c r="H67" s="40"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="37"/>
     </row>
     <row r="68" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
@@ -2555,9 +2555,9 @@
       <c r="C68" s="4"/>
       <c r="D68" s="5"/>
       <c r="E68" s="23"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="40"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="37"/>
     </row>
     <row r="69" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
@@ -2565,9 +2565,9 @@
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
       <c r="E69" s="23"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="39"/>
-      <c r="H69" s="40"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="37"/>
     </row>
     <row r="70" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
@@ -2575,9 +2575,9 @@
       <c r="C70" s="4"/>
       <c r="D70" s="5"/>
       <c r="E70" s="23"/>
-      <c r="F70" s="38"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="40"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="37"/>
     </row>
     <row r="71" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
@@ -2585,9 +2585,9 @@
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
       <c r="E71" s="23"/>
-      <c r="F71" s="38"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="40"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="37"/>
     </row>
     <row r="72" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
@@ -2595,9 +2595,9 @@
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
       <c r="E72" s="23"/>
-      <c r="F72" s="38"/>
-      <c r="G72" s="39"/>
-      <c r="H72" s="40"/>
+      <c r="F72" s="35"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="37"/>
     </row>
     <row r="73" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
@@ -2605,9 +2605,9 @@
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="23"/>
-      <c r="F73" s="38"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="40"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="36"/>
+      <c r="H73" s="37"/>
     </row>
     <row r="74" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
@@ -2615,9 +2615,9 @@
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="23"/>
-      <c r="F74" s="38"/>
-      <c r="G74" s="39"/>
-      <c r="H74" s="40"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="37"/>
     </row>
     <row r="75" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
@@ -2625,9 +2625,9 @@
       <c r="C75" s="4"/>
       <c r="D75" s="5"/>
       <c r="E75" s="23"/>
-      <c r="F75" s="38"/>
-      <c r="G75" s="39"/>
-      <c r="H75" s="40"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="37"/>
     </row>
     <row r="76" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
@@ -2635,9 +2635,9 @@
       <c r="C76" s="4"/>
       <c r="D76" s="5"/>
       <c r="E76" s="23"/>
-      <c r="F76" s="38"/>
-      <c r="G76" s="39"/>
-      <c r="H76" s="40"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="37"/>
     </row>
     <row r="77" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
@@ -2645,9 +2645,9 @@
       <c r="C77" s="4"/>
       <c r="D77" s="5"/>
       <c r="E77" s="23"/>
-      <c r="F77" s="38"/>
-      <c r="G77" s="39"/>
-      <c r="H77" s="40"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="37"/>
     </row>
     <row r="78" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
@@ -2655,9 +2655,9 @@
       <c r="C78" s="4"/>
       <c r="D78" s="5"/>
       <c r="E78" s="23"/>
-      <c r="F78" s="38"/>
-      <c r="G78" s="39"/>
-      <c r="H78" s="40"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="37"/>
     </row>
     <row r="79" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
@@ -2665,9 +2665,9 @@
       <c r="C79" s="4"/>
       <c r="D79" s="5"/>
       <c r="E79" s="23"/>
-      <c r="F79" s="38"/>
-      <c r="G79" s="39"/>
-      <c r="H79" s="40"/>
+      <c r="F79" s="35"/>
+      <c r="G79" s="36"/>
+      <c r="H79" s="37"/>
     </row>
     <row r="80" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
@@ -2675,9 +2675,9 @@
       <c r="C80" s="4"/>
       <c r="D80" s="5"/>
       <c r="E80" s="23"/>
-      <c r="F80" s="38"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="40"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="36"/>
+      <c r="H80" s="37"/>
     </row>
     <row r="81" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
@@ -2685,9 +2685,9 @@
       <c r="C81" s="4"/>
       <c r="D81" s="5"/>
       <c r="E81" s="23"/>
-      <c r="F81" s="38"/>
-      <c r="G81" s="39"/>
-      <c r="H81" s="40"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="36"/>
+      <c r="H81" s="37"/>
     </row>
     <row r="82" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
@@ -2695,9 +2695,9 @@
       <c r="C82" s="4"/>
       <c r="D82" s="5"/>
       <c r="E82" s="23"/>
-      <c r="F82" s="38"/>
-      <c r="G82" s="39"/>
-      <c r="H82" s="40"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="37"/>
     </row>
     <row r="83" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
@@ -2705,9 +2705,9 @@
       <c r="C83" s="4"/>
       <c r="D83" s="5"/>
       <c r="E83" s="23"/>
-      <c r="F83" s="38"/>
-      <c r="G83" s="39"/>
-      <c r="H83" s="40"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="37"/>
     </row>
     <row r="84" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
@@ -2715,9 +2715,9 @@
       <c r="C84" s="4"/>
       <c r="D84" s="5"/>
       <c r="E84" s="23"/>
-      <c r="F84" s="38"/>
-      <c r="G84" s="39"/>
-      <c r="H84" s="40"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="36"/>
+      <c r="H84" s="37"/>
     </row>
     <row r="85" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
@@ -2725,9 +2725,9 @@
       <c r="C85" s="4"/>
       <c r="D85" s="5"/>
       <c r="E85" s="23"/>
-      <c r="F85" s="38"/>
-      <c r="G85" s="39"/>
-      <c r="H85" s="40"/>
+      <c r="F85" s="35"/>
+      <c r="G85" s="36"/>
+      <c r="H85" s="37"/>
     </row>
     <row r="86" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
@@ -2735,9 +2735,9 @@
       <c r="C86" s="4"/>
       <c r="D86" s="5"/>
       <c r="E86" s="23"/>
-      <c r="F86" s="38"/>
-      <c r="G86" s="39"/>
-      <c r="H86" s="40"/>
+      <c r="F86" s="35"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="37"/>
     </row>
     <row r="87" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
@@ -2745,9 +2745,9 @@
       <c r="C87" s="4"/>
       <c r="D87" s="5"/>
       <c r="E87" s="23"/>
-      <c r="F87" s="38"/>
-      <c r="G87" s="39"/>
-      <c r="H87" s="40"/>
+      <c r="F87" s="35"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="37"/>
     </row>
     <row r="88" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
@@ -2755,9 +2755,9 @@
       <c r="C88" s="4"/>
       <c r="D88" s="5"/>
       <c r="E88" s="23"/>
-      <c r="F88" s="38"/>
-      <c r="G88" s="39"/>
-      <c r="H88" s="40"/>
+      <c r="F88" s="35"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="37"/>
     </row>
     <row r="89" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
@@ -2765,9 +2765,9 @@
       <c r="C89" s="4"/>
       <c r="D89" s="5"/>
       <c r="E89" s="23"/>
-      <c r="F89" s="38"/>
-      <c r="G89" s="39"/>
-      <c r="H89" s="40"/>
+      <c r="F89" s="35"/>
+      <c r="G89" s="36"/>
+      <c r="H89" s="37"/>
     </row>
     <row r="90" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
@@ -2775,9 +2775,9 @@
       <c r="C90" s="4"/>
       <c r="D90" s="5"/>
       <c r="E90" s="23"/>
-      <c r="F90" s="38"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="40"/>
+      <c r="F90" s="35"/>
+      <c r="G90" s="36"/>
+      <c r="H90" s="37"/>
     </row>
     <row r="91" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
@@ -2785,9 +2785,9 @@
       <c r="C91" s="4"/>
       <c r="D91" s="5"/>
       <c r="E91" s="23"/>
-      <c r="F91" s="38"/>
-      <c r="G91" s="39"/>
-      <c r="H91" s="40"/>
+      <c r="F91" s="35"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="37"/>
     </row>
     <row r="92" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
@@ -2795,9 +2795,9 @@
       <c r="C92" s="4"/>
       <c r="D92" s="5"/>
       <c r="E92" s="23"/>
-      <c r="F92" s="38"/>
-      <c r="G92" s="39"/>
-      <c r="H92" s="40"/>
+      <c r="F92" s="35"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="37"/>
     </row>
     <row r="93" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
@@ -2805,9 +2805,9 @@
       <c r="C93" s="4"/>
       <c r="D93" s="5"/>
       <c r="E93" s="23"/>
-      <c r="F93" s="38"/>
-      <c r="G93" s="39"/>
-      <c r="H93" s="40"/>
+      <c r="F93" s="35"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="37"/>
     </row>
     <row r="94" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
@@ -2815,9 +2815,9 @@
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
       <c r="E94" s="23"/>
-      <c r="F94" s="38"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="40"/>
+      <c r="F94" s="35"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="37"/>
     </row>
     <row r="95" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
@@ -2825,9 +2825,9 @@
       <c r="C95" s="4"/>
       <c r="D95" s="5"/>
       <c r="E95" s="23"/>
-      <c r="F95" s="38"/>
-      <c r="G95" s="39"/>
-      <c r="H95" s="40"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="37"/>
     </row>
     <row r="96" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
@@ -2835,9 +2835,9 @@
       <c r="C96" s="4"/>
       <c r="D96" s="5"/>
       <c r="E96" s="23"/>
-      <c r="F96" s="38"/>
-      <c r="G96" s="39"/>
-      <c r="H96" s="40"/>
+      <c r="F96" s="35"/>
+      <c r="G96" s="36"/>
+      <c r="H96" s="37"/>
     </row>
     <row r="97" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
@@ -2845,9 +2845,9 @@
       <c r="C97" s="4"/>
       <c r="D97" s="5"/>
       <c r="E97" s="23"/>
-      <c r="F97" s="38"/>
-      <c r="G97" s="39"/>
-      <c r="H97" s="40"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="37"/>
     </row>
     <row r="98" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
@@ -2855,9 +2855,9 @@
       <c r="C98" s="4"/>
       <c r="D98" s="5"/>
       <c r="E98" s="23"/>
-      <c r="F98" s="38"/>
-      <c r="G98" s="39"/>
-      <c r="H98" s="40"/>
+      <c r="F98" s="35"/>
+      <c r="G98" s="36"/>
+      <c r="H98" s="37"/>
     </row>
     <row r="99" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
@@ -2865,9 +2865,9 @@
       <c r="C99" s="4"/>
       <c r="D99" s="5"/>
       <c r="E99" s="23"/>
-      <c r="F99" s="38"/>
-      <c r="G99" s="39"/>
-      <c r="H99" s="40"/>
+      <c r="F99" s="35"/>
+      <c r="G99" s="36"/>
+      <c r="H99" s="37"/>
     </row>
     <row r="100" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
@@ -2875,103 +2875,13 @@
       <c r="C100" s="4"/>
       <c r="D100" s="5"/>
       <c r="E100" s="23"/>
-      <c r="F100" s="38"/>
-      <c r="G100" s="39"/>
-      <c r="H100" s="40"/>
+      <c r="F100" s="35"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="37"/>
     </row>
     <row r="101" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
@@ -2986,6 +2896,96 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3143,7 +3143,7 @@
       <c r="A2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="71">
+      <c r="B2" s="79">
         <v>41765</v>
       </c>
       <c r="C2" s="61"/>
@@ -3205,12 +3205,12 @@
       <c r="A8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="73"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="76"/>
     </row>
     <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
@@ -3238,12 +3238,12 @@
       <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="78"/>
     </row>
     <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3262,12 +3262,12 @@
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="77"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="72"/>
     </row>
     <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
@@ -3295,32 +3295,32 @@
       <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="79"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="74"/>
     </row>
     <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>